<commit_message>
Updated Learning Excel File and added File Zilla FTPs of Sagar Group by Manish
</commit_message>
<xml_diff>
--- a/I have to learn these.xlsx
+++ b/I have to learn these.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Topics to Learn" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="110">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -341,6 +341,25 @@
   </si>
   <si>
     <t>JWT / oAuth / oAuth2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7Q8_j9j1MZ8&amp;list=PLEMfWBGxd1ltBjtjLFawfMDkK9EM9GdW8</t>
+  </si>
+  <si>
+    <t>DevOps Bus Technology</t>
+  </si>
+  <si>
+    <t>DevOps
+Linux, AWS, Docker etc.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=WQoB2z67hvY&amp;list=PLDzeHZWIZsTryvtXdMr6rPh4IDexB5NIA</t>
+  </si>
+  <si>
+    <t>CodeHelp - by Babbar</t>
+  </si>
+  <si>
+    <t>Complete C++ Placement DSA Course</t>
   </si>
 </sst>
 </file>
@@ -730,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -1386,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1567,21 +1586,33 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75">
+    <row r="13" spans="1:4" ht="47.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75">
+      <c r="B13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="47.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="3">
@@ -1640,7 +1671,11 @@
       <c r="D21" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1"/>
+    <hyperlink ref="C14" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>